<commit_message>
add historical data & power energy sector
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_mongolia_transformation_v0.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_mongolia_transformation_v0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cffuentes\repos\ssp_mongolia\ssp_modeling\scenario_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5975D0AE-D322-43C3-AC84-A13EF3DF0C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B662F015-09BA-4BB8-9741-705460DB5186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$K$62</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1117,10 +1117,10 @@
     <t>transformation_waso_inc_recycling.yaml</t>
   </si>
   <si>
-    <t>strategy_NZ</t>
-  </si>
-  <si>
     <t>strategy_BaU</t>
+  </si>
+  <si>
+    <t>strategy_LEP</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,10 +1685,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>344</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="28" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,9 @@
       <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -3775,8 +3777,8 @@
     <sortCondition ref="B2:B62"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3786,7 +3788,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="175">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3797,8 +3799,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K62">
-    <cfRule type="colorScale" priority="160">
+  <conditionalFormatting sqref="J2:J62">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3810,6 +3812,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:K7">
+    <cfRule type="colorScale" priority="181">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K5 K7:K1048576">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="min"/>
@@ -3821,7 +3845,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="K2:K5 K7:K62">
+    <cfRule type="colorScale" priority="163">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3843,7 +3879,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J62">
+  <conditionalFormatting sqref="K6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3894,7 +3930,7 @@
       </c>
       <c r="F1" s="27" t="str">
         <f>main!K1</f>
-        <v>strategy_NZ</v>
+        <v>strategy_LEP</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4002,9 +4038,9 @@
         <f>IF(VLOOKUP($D6,main!$C$2:$K$62,8,FALSE)=0,"",VLOOKUP($D6,main!$C$2:$K$62,8,FALSE))</f>
         <v>1</v>
       </c>
-      <c r="F6" s="29" t="str">
+      <c r="F6" s="29">
         <f>IF(VLOOKUP($D6,main!$C$2:$K$62,9,FALSE)=0,"",VLOOKUP($D6,main!$C$2:$K$62,9,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>